<commit_message>
Fix some bugs and improve the performance
</commit_message>
<xml_diff>
--- a/Assets/ConfigTable/Test.xlsx
+++ b/Assets/ConfigTable/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Projects\ResearchGate\Assets\ConfigTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9614E0E-FCB2-421C-BB18-9F55610223D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CB2ED6-F07D-4B35-A79D-7A5CE209585D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -34,9 +34,6 @@
     <t>isTest</t>
   </si>
   <si>
-    <t>rate</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -58,43 +55,53 @@
     <t>float</t>
   </si>
   <si>
+    <t>rate factor</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>pear</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>cup</t>
+  </si>
+  <si>
+    <t>hat</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>factor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>bool</t>
-  </si>
-  <si>
-    <t>pig</t>
-  </si>
-  <si>
-    <t>rate factor</t>
-  </si>
-  <si>
-    <t>apple</t>
-  </si>
-  <si>
-    <t>dog</t>
-  </si>
-  <si>
-    <t>banana</t>
-  </si>
-  <si>
-    <t>pen</t>
-  </si>
-  <si>
-    <t>pear</t>
-  </si>
-  <si>
-    <t>chair</t>
-  </si>
-  <si>
-    <t>cup</t>
-  </si>
-  <si>
-    <t>hat</t>
-  </si>
-  <si>
-    <t>mouse</t>
-  </si>
-  <si>
-    <t>enum | red, green, blue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>green</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">enum | red, green, blue, </t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1061,12 +1068,12 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="20.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1083,39 +1090,39 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1123,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>1.2</v>
@@ -1136,10 +1143,10 @@
         <v>2.76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1147,7 +1154,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>3.4</v>
@@ -1160,7 +1167,7 @@
         <v>7.8199999999999994</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="5">
         <v>2.2999999999999998</v>
@@ -1171,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>5.3</v>
@@ -1184,7 +1191,7 @@
         <v>12.19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1192,7 +1199,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>7.3</v>
@@ -1205,7 +1212,7 @@
         <v>16.79</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1213,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>1.5</v>
@@ -1226,7 +1233,7 @@
         <v>3.4499999999999997</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1234,7 +1241,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>5.09</v>
@@ -1247,7 +1254,7 @@
         <v>11.706999999999999</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1255,7 +1262,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>5.54</v>
@@ -1268,7 +1275,7 @@
         <v>12.741999999999999</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1276,7 +1283,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1">
         <v>5.99</v>
@@ -1289,7 +1296,7 @@
         <v>13.776999999999999</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1297,7 +1304,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1">
         <v>6.44</v>
@@ -1310,7 +1317,7 @@
         <v>14.811999999999999</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1318,7 +1325,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
         <v>5.7</v>
@@ -1331,16 +1338,11 @@
         <v>13.11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F12" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$I$1:$K$1</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix compile and reload bug
</commit_message>
<xml_diff>
--- a/Assets/ConfigTable/Test.xlsx
+++ b/Assets/ConfigTable/Test.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20358"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Projects\ResearchGate\Assets\ConfigTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity Projects\ResearchGate\Assets\ConfigTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CB2ED6-F07D-4B35-A79D-7A5CE209585D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -93,22 +92,22 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>green</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>gate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">enum | red, green, blue, </t>
+    <t>red</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum | red, green, blue</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1064,19 +1063,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="26.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1125,12 +1124,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>1.2</v>
@@ -1143,13 +1142,13 @@
         <v>2.76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1236,7 +1235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1257,7 +1256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1278,7 +1277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1299,7 +1298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Optimize the parsing process from two-passe to one and refactor the strcuture of table compiler
</commit_message>
<xml_diff>
--- a/Assets/ConfigTable/Test.xlsx
+++ b/Assets/ConfigTable/Test.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -52,9 +53,6 @@
   </si>
   <si>
     <t>float</t>
-  </si>
-  <si>
-    <t>rate factor</t>
   </si>
   <si>
     <t>apple</t>
@@ -101,6 +99,14 @@
   </si>
   <si>
     <t>enum | red, green, blue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rate factor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1066,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1089,7 +1095,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -1115,13 +1121,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1129,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1">
         <v>1.2</v>
@@ -1142,10 +1148,10 @@
         <v>2.76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1153,7 +1159,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>3.4</v>
@@ -1177,7 +1183,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>5.3</v>
@@ -1198,7 +1204,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>7.3</v>
@@ -1219,7 +1225,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>1.5</v>
@@ -1240,7 +1246,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>5.09</v>
@@ -1261,7 +1267,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>5.54</v>
@@ -1282,7 +1288,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
         <v>5.99</v>
@@ -1303,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
         <v>6.44</v>
@@ -1324,7 +1330,283 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>13.11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f>$I$4*C3</f>
+        <v>2.76</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E12" si="0">$I$4*C4</f>
+        <v>7.8199999999999994</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>12.19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>16.79</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4499999999999997</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5.09</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>11.706999999999999</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5.54</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>12.741999999999999</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>13.776999999999999</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.44</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>14.811999999999999</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C12" s="1">
         <v>5.7</v>

</xml_diff>

<commit_message>
Start the compiling and reloading process only when files got changed
</commit_message>
<xml_diff>
--- a/Assets/ConfigTable/Test.xlsx
+++ b/Assets/ConfigTable/Test.xlsx
@@ -13,14 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -86,23 +85,27 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>gate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>enum | red, green, blue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rate factor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>red</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>enum | red, green, blue</t>
+    <t>blue</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>rate factor</t>
+    <t>green</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1073,7 +1076,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1121,13 +1124,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1135,23 +1138,23 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1">
         <v>1.2</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
         <f>$I$4*C3</f>
         <v>2.76</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1238,7 +1241,7 @@
         <v>3.4499999999999997</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1301,7 +1304,7 @@
         <v>13.776999999999999</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1328,282 +1331,6 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1">
-        <v>5.7</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>13.11</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
-  <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <f>$I$4*C3</f>
-        <v>2.76</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" ref="E4:E12" si="0">$I$4*C4</f>
-        <v>7.8199999999999994</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5.3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>12.19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7.3</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>16.79</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4499999999999997</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5.09</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>11.706999999999999</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5.54</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>12.741999999999999</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5.99</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>13.776999999999999</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6.44</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>14.811999999999999</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Exclude table compiler scripts from building
</commit_message>
<xml_diff>
--- a/Assets/ConfigTable/Test.xlsx
+++ b/Assets/ConfigTable/Test.xlsx
@@ -733,7 +733,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -751,6 +751,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1076,12 +1079,12 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1144,7 +1147,7 @@
         <v>1.2</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <f>$I$4*C3</f>
@@ -1245,107 +1248,107 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="6">
         <v>5.09</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>11.706999999999999</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="6">
         <v>5.54</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>12.741999999999999</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="6">
         <v>5.99</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <f t="shared" si="0"/>
         <v>13.776999999999999</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="6">
         <v>6.44</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="6">
         <v>0</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <f t="shared" si="0"/>
         <v>14.811999999999999</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="6">
         <v>5.7</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="6">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="6">
         <f t="shared" si="0"/>
         <v>13.11</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>